<commit_message>
macro specs improves forecasts
</commit_message>
<xml_diff>
--- a/Results/Forecasting Results.xlsx
+++ b/Results/Forecasting Results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>Dynamic Factor Model</t>
   </si>
@@ -59,7 +59,22 @@
     <t>DFM Without Unemployment</t>
   </si>
   <si>
-    <t>DFM With Unemployment</t>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>Dynamic Factor Model Including Unemployment (Lag - 2)</t>
+  </si>
+  <si>
+    <t>Dynamic Factor Model Including Unemployment (restrictions following macroeconomic relations)</t>
+  </si>
+  <si>
+    <t>Dynamic Factor Model Including Unemployment (without restrictions)</t>
+  </si>
+  <si>
+    <t>Short Rate (Bernanke)</t>
+  </si>
+  <si>
+    <t>Short Rate (estimated)</t>
   </si>
 </sst>
 </file>
@@ -134,7 +149,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -144,8 +159,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -161,16 +192,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1018,585 +1074,874 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="R19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="1"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+      <c r="C21" s="10">
         <v>2</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="8" t="s">
+      <c r="D21" s="10">
         <v>3</v>
       </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="E21" s="10">
+        <v>4</v>
+      </c>
+      <c r="F21" s="10">
+        <v>8</v>
+      </c>
+      <c r="G21" s="10">
+        <v>12</v>
+      </c>
+      <c r="H21" s="10">
+        <v>16</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" s="10">
+        <v>1</v>
+      </c>
+      <c r="T21" s="10">
         <v>2</v>
       </c>
-      <c r="D22">
+      <c r="U21" s="10">
         <v>3</v>
       </c>
-      <c r="E22">
+      <c r="V21" s="10">
         <v>4</v>
       </c>
-      <c r="F22">
+      <c r="W21" s="10">
         <v>8</v>
       </c>
-      <c r="G22">
+      <c r="X21" s="10">
         <v>12</v>
       </c>
-      <c r="H22">
+      <c r="Y21" s="10">
         <v>16</v>
       </c>
-      <c r="J22" s="4">
-        <v>1</v>
-      </c>
-      <c r="K22" s="4">
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="12">
+        <v>1.0048999999999999</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1.0054000000000001</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="G22" s="12">
+        <v>1.0003</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1.0099</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="R22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="S22" s="12">
+        <v>1.0044999999999999</v>
+      </c>
+      <c r="T22" s="12">
+        <v>1.0111000000000001</v>
+      </c>
+      <c r="U22" s="12">
+        <v>1.0088999999999999</v>
+      </c>
+      <c r="V22" s="12">
+        <v>1.0348999999999999</v>
+      </c>
+      <c r="W22" s="12">
+        <v>1.0159</v>
+      </c>
+      <c r="X22" s="12">
+        <v>1.0866</v>
+      </c>
+      <c r="Y22" s="12">
+        <v>1.1120000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="12">
+        <v>1.2677</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1.1817</v>
+      </c>
+      <c r="D23" s="12">
+        <v>1.1095999999999999</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1.0538000000000001</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.98570000000000002</v>
+      </c>
+      <c r="G23" s="12">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="H23" s="12">
+        <v>1.0390999999999999</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="R23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="S23" s="12">
+        <v>1.3151999999999999</v>
+      </c>
+      <c r="T23" s="12">
+        <v>1.2441</v>
+      </c>
+      <c r="U23" s="12">
+        <v>1.1738999999999999</v>
+      </c>
+      <c r="V23" s="12">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="W23" s="12">
+        <v>1.079</v>
+      </c>
+      <c r="X23" s="12">
+        <v>1.1191</v>
+      </c>
+      <c r="Y23" s="12">
+        <v>1.1560999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1.0397000000000001</v>
+      </c>
+      <c r="C24" s="12">
+        <v>1.0409999999999999</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1.0427</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1.0664</v>
+      </c>
+      <c r="F24" s="12">
+        <v>1.0676000000000001</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0.97030000000000005</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0.996</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="R24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="S24" s="12">
+        <v>1.0744</v>
+      </c>
+      <c r="T24" s="12">
+        <v>1.0636000000000001</v>
+      </c>
+      <c r="U24" s="12">
+        <v>1.1657</v>
+      </c>
+      <c r="V24" s="12">
+        <v>1.1958</v>
+      </c>
+      <c r="W24" s="12">
+        <v>1.1879</v>
+      </c>
+      <c r="X24" s="12">
+        <v>1.1037999999999999</v>
+      </c>
+      <c r="Y24" s="12">
+        <v>1.1483000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1.0378000000000001</v>
+      </c>
+      <c r="C25" s="12">
+        <v>1.0221</v>
+      </c>
+      <c r="D25" s="12">
+        <v>1.0347</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.0364</v>
+      </c>
+      <c r="F25" s="12">
+        <v>1.0384</v>
+      </c>
+      <c r="G25" s="12">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="H25" s="12">
+        <v>1.0310999999999999</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="R25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="S25" s="12">
+        <v>1.0707</v>
+      </c>
+      <c r="T25" s="12">
+        <v>1.054</v>
+      </c>
+      <c r="U25" s="12">
+        <v>1.0821000000000001</v>
+      </c>
+      <c r="V25" s="12">
+        <v>1.1017999999999999</v>
+      </c>
+      <c r="W25" s="12">
+        <v>1.1237999999999999</v>
+      </c>
+      <c r="X25" s="12">
+        <v>1.1398999999999999</v>
+      </c>
+      <c r="Y25" s="12">
+        <v>1.0941000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
         <v>2</v>
       </c>
-      <c r="L22" s="4">
+      <c r="D27" s="4">
         <v>3</v>
       </c>
-      <c r="M22" s="4">
+      <c r="E27" s="4">
         <v>4</v>
       </c>
-      <c r="N22" s="4">
+      <c r="F27" s="4">
         <v>8</v>
       </c>
-      <c r="O22" s="4">
+      <c r="G27" s="4">
         <v>12</v>
       </c>
-      <c r="P22" s="4">
+      <c r="H27" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="R27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="S27" s="4">
+        <v>1</v>
+      </c>
+      <c r="T27" s="4">
+        <v>2</v>
+      </c>
+      <c r="U27" s="4">
+        <v>3</v>
+      </c>
+      <c r="V27" s="4">
+        <v>4</v>
+      </c>
+      <c r="W27" s="4">
+        <v>8</v>
+      </c>
+      <c r="X27" s="4">
+        <v>12</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="12">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0.98550000000000004</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="H28" s="12">
+        <v>0.91649999999999998</v>
+      </c>
+      <c r="R28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3">
-        <v>1.0048999999999999</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1.0054000000000001</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="G23" s="3">
-        <v>1.0003</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1.0099</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3">
-        <v>0.98640000000000005</v>
-      </c>
-      <c r="K23" s="3">
+      <c r="S28" s="12">
+        <v>0.97950000000000004</v>
+      </c>
+      <c r="T28" s="12">
+        <v>0.97819999999999996</v>
+      </c>
+      <c r="U28" s="12">
+        <v>0.99019999999999997</v>
+      </c>
+      <c r="V28" s="12">
+        <v>1.0037</v>
+      </c>
+      <c r="W28" s="12">
+        <v>1.0246</v>
+      </c>
+      <c r="X28" s="12">
+        <v>1.0555000000000001</v>
+      </c>
+      <c r="Y28" s="12">
+        <v>1.0859000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1.3338000000000001</v>
+      </c>
+      <c r="C29" s="12">
+        <v>1.2343999999999999</v>
+      </c>
+      <c r="D29" s="12">
+        <v>1.1458999999999999</v>
+      </c>
+      <c r="E29" s="12">
+        <v>1.0801000000000001</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0.93220000000000003</v>
+      </c>
+      <c r="R29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="S29" s="12">
+        <v>1.3436999999999999</v>
+      </c>
+      <c r="T29" s="12">
+        <v>1.2801</v>
+      </c>
+      <c r="U29" s="12">
+        <v>1.2236</v>
+      </c>
+      <c r="V29" s="12">
+        <v>1.1673</v>
+      </c>
+      <c r="W29" s="12">
+        <v>1.1124000000000001</v>
+      </c>
+      <c r="X29" s="12">
+        <v>1.1486000000000001</v>
+      </c>
+      <c r="Y29" s="12">
+        <v>1.1651</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="12">
+        <v>1.0284</v>
+      </c>
+      <c r="C30" s="12">
+        <v>1.0676000000000001</v>
+      </c>
+      <c r="D30" s="12">
+        <v>1.0958000000000001</v>
+      </c>
+      <c r="E30" s="12">
+        <v>1.0939000000000001</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0.95330000000000004</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.93089999999999995</v>
+      </c>
+      <c r="H30" s="12">
+        <v>0.92820000000000003</v>
+      </c>
+      <c r="R30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="S30" s="12">
+        <v>1.0535000000000001</v>
+      </c>
+      <c r="T30" s="12">
+        <v>1.1207</v>
+      </c>
+      <c r="U30" s="12">
+        <v>1.204</v>
+      </c>
+      <c r="V30" s="12">
+        <v>1.2130000000000001</v>
+      </c>
+      <c r="W30" s="12">
+        <v>1.0967</v>
+      </c>
+      <c r="X30" s="12">
+        <v>1.0065</v>
+      </c>
+      <c r="Y30" s="12">
+        <v>1.0612999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="12">
+        <v>1.0258</v>
+      </c>
+      <c r="C31" s="12">
+        <v>1.0304</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1.0293000000000001</v>
+      </c>
+      <c r="E31" s="12">
+        <v>1.0227999999999999</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="G31" s="12">
+        <v>0.97189999999999999</v>
+      </c>
+      <c r="H31" s="12">
+        <v>0.9728</v>
+      </c>
+      <c r="R31" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="S31" s="12">
+        <v>1.0601</v>
+      </c>
+      <c r="T31" s="12">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="U31" s="12">
+        <v>1.0857000000000001</v>
+      </c>
+      <c r="V31" s="12">
+        <v>1.0803</v>
+      </c>
+      <c r="W31" s="12">
+        <v>1.0831</v>
+      </c>
+      <c r="X31" s="12">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="Y31" s="12">
+        <v>1.1192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="10">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10">
+        <v>2</v>
+      </c>
+      <c r="D34" s="10">
+        <v>3</v>
+      </c>
+      <c r="E34" s="10">
+        <v>4</v>
+      </c>
+      <c r="F34" s="10">
+        <v>8</v>
+      </c>
+      <c r="G34" s="10">
+        <v>12</v>
+      </c>
+      <c r="H34" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1.0282</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1.0275000000000001</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.91320000000000001</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.80569999999999997</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.73740000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1.2867999999999999</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1.1951000000000001</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.1323000000000001</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1.0763</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.85660000000000003</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1.0024</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.0006999999999999</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1.0043</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.99019999999999997</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0.99439999999999995</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.95740000000000003</v>
+      </c>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.9294</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.8891</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.86140000000000005</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.8377</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.82520000000000004</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4">
+        <v>2</v>
+      </c>
+      <c r="D40" s="4">
+        <v>3</v>
+      </c>
+      <c r="E40" s="4">
+        <v>4</v>
+      </c>
+      <c r="F40" s="4">
+        <v>8</v>
+      </c>
+      <c r="G40" s="4">
+        <v>12</v>
+      </c>
+      <c r="H40" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="12">
+        <v>1.0034000000000001</v>
+      </c>
+      <c r="C41" s="12">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0.97370000000000001</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0.94430000000000003</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0.83279999999999998</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.7218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="12">
+        <v>1.3396999999999999</v>
+      </c>
+      <c r="C42" s="12">
+        <v>1.2588999999999999</v>
+      </c>
+      <c r="D42" s="12">
+        <v>1.1895</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1.1231</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.95209999999999995</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0.86429999999999996</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.78300000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="12">
+        <v>0.99909999999999999</v>
+      </c>
+      <c r="C43" s="12">
+        <v>0.998</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1.0001</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="G43" s="12">
         <v>0.98550000000000004</v>
       </c>
-      <c r="L23" s="3">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="M23" s="3">
-        <v>0.98640000000000005</v>
-      </c>
-      <c r="N23" s="3">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="O23" s="3">
-        <v>0.93259999999999998</v>
-      </c>
-      <c r="P23" s="3">
-        <v>0.91649999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1.2677</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1.1817</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1.1095999999999999</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1.0538000000000001</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.98570000000000002</v>
-      </c>
-      <c r="G24" s="3">
-        <v>1.0169999999999999</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1.0390999999999999</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3">
-        <v>1.3338000000000001</v>
-      </c>
-      <c r="K24" s="3">
-        <v>1.2343999999999999</v>
-      </c>
-      <c r="L24" s="3">
-        <v>1.1458999999999999</v>
-      </c>
-      <c r="M24" s="3">
-        <v>1.0801000000000001</v>
-      </c>
-      <c r="N24" s="3">
-        <v>0.99050000000000005</v>
-      </c>
-      <c r="O24" s="3">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="P24" s="3">
-        <v>0.93220000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1.0397000000000001</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1.0409999999999999</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1.0427</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1.0664</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1.0676000000000001</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0.97030000000000005</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.996</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3">
-        <v>1.0284</v>
-      </c>
-      <c r="K25" s="3">
-        <v>1.0676000000000001</v>
-      </c>
-      <c r="L25" s="3">
-        <v>1.0958000000000001</v>
-      </c>
-      <c r="M25" s="3">
-        <v>1.0939000000000001</v>
-      </c>
-      <c r="N25" s="3">
-        <v>0.95330000000000004</v>
-      </c>
-      <c r="O25" s="3">
-        <v>0.93089999999999995</v>
-      </c>
-      <c r="P25" s="3">
-        <v>0.92820000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="H43" s="3">
+        <v>0.95840000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="3">
-        <v>1.0378000000000001</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1.0221</v>
-      </c>
-      <c r="D26" s="3">
-        <v>1.0347</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1.0364</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1.0384</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1.0309999999999999</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1.0310999999999999</v>
-      </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3">
-        <v>1.0258</v>
-      </c>
-      <c r="K26" s="3">
-        <v>1.0304</v>
-      </c>
-      <c r="L26" s="3">
-        <v>1.0293000000000001</v>
-      </c>
-      <c r="M26" s="3">
-        <v>1.0227999999999999</v>
-      </c>
-      <c r="N26" s="3">
-        <v>0.99390000000000001</v>
-      </c>
-      <c r="O26" s="3">
-        <v>0.97189999999999999</v>
-      </c>
-      <c r="P26" s="3">
-        <v>0.9728</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>4</v>
-      </c>
-      <c r="F30">
-        <v>8</v>
-      </c>
-      <c r="G30">
-        <v>12</v>
-      </c>
-      <c r="H30">
-        <v>16</v>
-      </c>
-      <c r="J30" s="4">
-        <v>1</v>
-      </c>
-      <c r="K30" s="4">
-        <v>2</v>
-      </c>
-      <c r="L30" s="4">
-        <v>3</v>
-      </c>
-      <c r="M30" s="4">
-        <v>4</v>
-      </c>
-      <c r="N30" s="4">
-        <v>8</v>
-      </c>
-      <c r="O30" s="4">
-        <v>12</v>
-      </c>
-      <c r="P30" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1.0044999999999999</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1.0111000000000001</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1.0088999999999999</v>
-      </c>
-      <c r="E31" s="3">
-        <v>1.0348999999999999</v>
-      </c>
-      <c r="F31" s="3">
-        <v>1.0159</v>
-      </c>
-      <c r="G31" s="3">
-        <v>1.0866</v>
-      </c>
-      <c r="H31" s="3">
-        <v>1.1120000000000001</v>
-      </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3">
-        <v>0.97950000000000004</v>
-      </c>
-      <c r="K31" s="3">
-        <v>0.97819999999999996</v>
-      </c>
-      <c r="L31" s="3">
-        <v>0.99019999999999997</v>
-      </c>
-      <c r="M31" s="3">
-        <v>1.0037</v>
-      </c>
-      <c r="N31" s="3">
-        <v>1.0246</v>
-      </c>
-      <c r="O31" s="3">
-        <v>1.0555000000000001</v>
-      </c>
-      <c r="P31" s="3">
-        <v>1.0859000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1.3151999999999999</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1.2441</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1.1738999999999999</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1.079</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1.1191</v>
-      </c>
-      <c r="H32" s="3">
-        <v>1.1560999999999999</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3">
-        <v>1.3436999999999999</v>
-      </c>
-      <c r="K32" s="3">
-        <v>1.2801</v>
-      </c>
-      <c r="L32" s="3">
-        <v>1.2236</v>
-      </c>
-      <c r="M32" s="3">
-        <v>1.1673</v>
-      </c>
-      <c r="N32" s="3">
-        <v>1.1124000000000001</v>
-      </c>
-      <c r="O32" s="3">
-        <v>1.1486000000000001</v>
-      </c>
-      <c r="P32" s="3">
-        <v>1.1651</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1.0744</v>
-      </c>
-      <c r="C33" s="3">
-        <v>1.0636000000000001</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1.1657</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1.1958</v>
-      </c>
-      <c r="F33" s="3">
-        <v>1.1879</v>
-      </c>
-      <c r="G33" s="3">
-        <v>1.1037999999999999</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1.1483000000000001</v>
-      </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3">
-        <v>1.0535000000000001</v>
-      </c>
-      <c r="K33" s="3">
-        <v>1.1207</v>
-      </c>
-      <c r="L33" s="3">
-        <v>1.204</v>
-      </c>
-      <c r="M33" s="3">
-        <v>1.2130000000000001</v>
-      </c>
-      <c r="N33" s="3">
-        <v>1.0967</v>
-      </c>
-      <c r="O33" s="3">
-        <v>1.0065</v>
-      </c>
-      <c r="P33" s="3">
-        <v>1.0612999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1.0707</v>
-      </c>
-      <c r="C34" s="3">
-        <v>1.054</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1.0821000000000001</v>
-      </c>
-      <c r="E34" s="3">
-        <v>1.1017999999999999</v>
-      </c>
-      <c r="F34" s="3">
-        <v>1.1237999999999999</v>
-      </c>
-      <c r="G34" s="3">
-        <v>1.1398999999999999</v>
-      </c>
-      <c r="H34" s="3">
-        <v>1.0941000000000001</v>
-      </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3">
-        <v>1.0601</v>
-      </c>
-      <c r="K34" s="3">
-        <v>1.0780000000000001</v>
-      </c>
-      <c r="L34" s="3">
-        <v>1.0857000000000001</v>
-      </c>
-      <c r="M34" s="3">
-        <v>1.0803</v>
-      </c>
-      <c r="N34" s="3">
-        <v>1.0831</v>
-      </c>
-      <c r="O34" s="3">
-        <v>1.1040000000000001</v>
-      </c>
-      <c r="P34" s="3">
-        <v>1.1192</v>
+      <c r="B44" s="12">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="C44" s="12">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0.90539999999999998</v>
+      </c>
+      <c r="E44" s="12">
+        <v>0.87239999999999995</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0.83169999999999999</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0.80149999999999999</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0.77280000000000004</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="11">
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B28:P28"/>
+    <mergeCell ref="R19:Y19"/>
+    <mergeCell ref="A19:H19"/>
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B29:H29"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="J12:P12"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="A32:H32"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B11:P11"/>
-    <mergeCell ref="B20:P20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>